<commit_message>
add create flow page
</commit_message>
<xml_diff>
--- a/Wiki/Nextjs.xlsx
+++ b/Wiki/Nextjs.xlsx
@@ -5,23 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Calamari\calamari-app\Wiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC5261F-59F8-4383-B155-2B0B40699179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1487BA-06C8-41EF-9EB5-18F90DD7230E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31110" yWindow="150" windowWidth="17310" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compare React vs Nextjs" sheetId="1" r:id="rId1"/>
-    <sheet name="Q&amp;A" sheetId="2" r:id="rId2"/>
+    <sheet name="Links" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>COMPARE</t>
   </si>
@@ -397,33 +397,6 @@
   <si>
     <t>sau khi hydration nếu query không phải rỗng thì sẽ trigger update
 =&gt; nếu dùng useEffect check query available</t>
-  </si>
-  <si>
-    <t>1.Cách lúc load page lần đầu trả về cả html và data như thế nào</t>
-  </si>
-  <si>
-    <t>2.Sau đó get data khác thì server trả về thế nào</t>
-  </si>
-  <si>
-    <t>3. Thử các cách gọi api xem thay đổi như thế nào</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. List ra các so sánh giữa reactjs và nextjs </t>
-  </si>
-  <si>
-    <t>5. Tạo 1 file flow các tính năng bên FE</t>
-  </si>
-  <si>
-    <t>Lúc build bằng SSG thì đã fetch data nên khi có request sẽ trả về cả HTML và data</t>
-  </si>
-  <si>
-    <t>SSG: get page mới thì trả về notfound</t>
-  </si>
-  <si>
-    <t>SSR: get page mới chưa build thì sẽ build rồi trả về</t>
-  </si>
-  <si>
-    <t>CSR: fetch data ở client</t>
   </si>
   <si>
     <r>
@@ -688,17 +661,30 @@
 không phảil fullpage reload
 fetch thêm thông tin, thực hiện chuyển đổi các trang</t>
   </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/spreadsheets/d/15ikXz-VNvKNgOZzUKyo1_VSr93pZaOK_wDT252eTwno/edit#gid=0 </t>
+  </si>
+  <si>
+    <t>file flow các tính năng bên FE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -857,11 +843,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -876,40 +862,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -918,19 +902,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1209,15 +1195,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="77" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="83.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="73.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="34" style="4" customWidth="1"/>
     <col min="5" max="5" width="9.109375" style="5"/>
     <col min="6" max="6" width="82.44140625" style="5" customWidth="1"/>
@@ -1237,12 +1223,12 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1253,25 +1239,25 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8">
-      <c r="A3" s="13"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="13"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="14"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1282,7 +1268,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="13"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1291,7 +1277,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="13"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="9" t="s">
         <v>16</v>
       </c>
@@ -1300,7 +1286,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="14"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1323,21 +1309,21 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="57.6">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="86.4">
-      <c r="A12" s="13"/>
+      <c r="B11" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="192" customHeight="1">
+      <c r="A12" s="21"/>
       <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="86.4">
-      <c r="A13" s="14"/>
+    <row r="13" spans="1:6" ht="173.4" customHeight="1">
+      <c r="A13" s="22"/>
       <c r="B13" s="10" t="s">
         <v>26</v>
       </c>
@@ -1359,7 +1345,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="158.4">
+    <row r="15" spans="1:6" ht="144">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1371,24 +1357,24 @@
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>58</v>
+      <c r="B16" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="276.60000000000002" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>57</v>
+      <c r="B17" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="409.5" customHeight="1">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>56</v>
+      <c r="B18" s="16" t="s">
+        <v>47</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="4" t="s">
@@ -1396,7 +1382,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="46.8" customHeight="1">
-      <c r="A19" s="16"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="17"/>
       <c r="C19" s="19"/>
     </row>
@@ -1412,7 +1398,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="81.599999999999994" customHeight="1">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1420,9 +1406,9 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="186.6" customHeight="1">
-      <c r="A22" s="14"/>
-      <c r="B22" s="21" t="s">
-        <v>59</v>
+      <c r="A22" s="22"/>
+      <c r="B22" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="86.4">
@@ -1444,13 +1430,13 @@
     <row r="25" spans="1:4" ht="30.6" customHeight="1"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1463,67 +1449,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28A33A0-0A38-424F-B114-B8E1F9669D30}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="15" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="24" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A17" r:id="rId1" xr:uid="{6C315925-0091-4619-A868-692AD2148E36}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6C315925-0091-4619-A868-692AD2148E36}"/>
+    <hyperlink ref="A3" r:id="rId2" location="gid=0 " xr:uid="{774DCA72-A272-4638-B690-5EE702FBAF50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>